<commit_message>
recommitting to try to fix merging issues
</commit_message>
<xml_diff>
--- a/Data/Detroit Deaths.xlsx
+++ b/Data/Detroit Deaths.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timmymiller/Library/Mobile Documents/com~apple~CloudDocs/Stat 300/STAT-300-Fa20/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A249D163-5FA4-3744-8AA0-E47EE27E4D7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE2FD8B2-FA19-9543-84FB-A564BFCB6696}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{97C615E2-605A-AE44-B0FB-D0C0A75923DB}"/>
+    <workbookView xWindow="11280" yWindow="1660" windowWidth="10000" windowHeight="14440" xr2:uid="{97C615E2-605A-AE44-B0FB-D0C0A75923DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>ZIP Code</t>
   </si>
@@ -41,7 +41,7 @@
     <t>Deaths_per_HundThou</t>
   </si>
   <si>
-    <t>?</t>
+    <t>Cases_per_HundThou</t>
   </si>
 </sst>
 </file>
@@ -393,244 +393,274 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C61DCE7-7026-C947-8C68-A5D4929B7D05}">
-  <dimension ref="A2:B29"/>
+  <dimension ref="A2:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B29"/>
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>48201</v>
       </c>
       <c r="B3">
         <v>209</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3">
+        <v>1885</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>48202</v>
       </c>
       <c r="B4">
         <v>193</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4">
+        <v>1884</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>48203</v>
       </c>
       <c r="B5">
         <v>142</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>48204</v>
       </c>
       <c r="B6">
         <v>204</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6">
+        <v>1735</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>48205</v>
       </c>
       <c r="B7">
         <v>163</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7">
+        <v>1566</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>48206</v>
       </c>
       <c r="B8">
         <v>124</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8">
+        <v>1528</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>48207</v>
       </c>
       <c r="B9">
         <v>525</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9">
+        <v>2893</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>48208</v>
       </c>
       <c r="B10">
         <v>283</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10">
+        <v>2155</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11">
-        <v>48209</v>
-      </c>
-      <c r="B11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
+        <v>48210</v>
+      </c>
+      <c r="B11">
+        <v>67</v>
+      </c>
+      <c r="C11">
+        <v>1959</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12">
-        <v>48210</v>
+        <v>48211</v>
       </c>
       <c r="B12">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
+        <v>265</v>
+      </c>
+      <c r="C12">
+        <v>2849</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13">
-        <v>48211</v>
+        <v>48213</v>
       </c>
       <c r="B13">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
+        <v>249</v>
+      </c>
+      <c r="C13">
+        <v>1593</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14">
-        <v>48212</v>
-      </c>
-      <c r="B14" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
+        <v>48214</v>
+      </c>
+      <c r="B14">
+        <v>341</v>
+      </c>
+      <c r="C14">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15">
-        <v>48213</v>
+        <v>48215</v>
       </c>
       <c r="B15">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
+        <v>185</v>
+      </c>
+      <c r="C15">
+        <v>1646</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16">
-        <v>48214</v>
+        <v>48219</v>
       </c>
       <c r="B16">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+        <v>299</v>
+      </c>
+      <c r="C16">
+        <v>2211</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17">
-        <v>48215</v>
+        <v>48221</v>
       </c>
       <c r="B17">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+        <v>223</v>
+      </c>
+      <c r="C17">
+        <v>2153</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18">
-        <v>48216</v>
-      </c>
-      <c r="B18" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
+        <v>48223</v>
+      </c>
+      <c r="B18">
+        <v>153</v>
+      </c>
+      <c r="C18">
+        <v>1718</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19">
-        <v>48217</v>
-      </c>
-      <c r="B19" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
+        <v>48224</v>
+      </c>
+      <c r="B19">
+        <v>224</v>
+      </c>
+      <c r="C19">
+        <v>1770</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20">
-        <v>48219</v>
+        <v>48227</v>
       </c>
       <c r="B20">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
+        <v>194</v>
+      </c>
+      <c r="C20">
+        <v>1817</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21">
-        <v>48221</v>
+        <v>48228</v>
       </c>
       <c r="B21">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
+        <v>160</v>
+      </c>
+      <c r="C21">
+        <v>1958</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22">
-        <v>48223</v>
+        <v>48234</v>
       </c>
       <c r="B22">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
+        <v>204</v>
+      </c>
+      <c r="C22">
+        <v>1610</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23">
-        <v>48224</v>
+        <v>48235</v>
       </c>
       <c r="B23">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
+        <v>381</v>
+      </c>
+      <c r="C23">
+        <v>2707</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24">
-        <v>48226</v>
-      </c>
-      <c r="B24" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25">
-        <v>48227</v>
-      </c>
-      <c r="B25">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26">
-        <v>48228</v>
-      </c>
-      <c r="B26">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27">
-        <v>48234</v>
-      </c>
-      <c r="B27">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28">
-        <v>48235</v>
-      </c>
-      <c r="B28">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29">
         <v>48238</v>
       </c>
-      <c r="B29">
+      <c r="B24">
         <v>121</v>
       </c>
+      <c r="C24">
+        <v>1490</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:B29">
-    <sortCondition ref="A3:A29"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:B24">
+    <sortCondition ref="A3:A24"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>